<commit_message>
Work on CPU design
</commit_message>
<xml_diff>
--- a/documentation/OP_CODE.xlsx
+++ b/documentation/OP_CODE.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="81">
   <si>
     <t>OPCODE List</t>
   </si>
@@ -76,7 +76,7 @@
     <t>OR</t>
   </si>
   <si>
-    <t>MOVRET</t>
+    <t>JAL</t>
   </si>
   <si>
     <t>Copy return address from PC to reg</t>
@@ -103,94 +103,85 @@
     <t>NOT</t>
   </si>
   <si>
-    <t>ADDC</t>
+    <t>SUB</t>
+  </si>
+  <si>
+    <t>1001</t>
+  </si>
+  <si>
+    <t>SUBI</t>
+  </si>
+  <si>
+    <t>CMP</t>
   </si>
   <si>
     <t>0111</t>
   </si>
   <si>
-    <t>ADDCU</t>
+    <t>ALSH</t>
+  </si>
+  <si>
+    <t>CMPI</t>
+  </si>
+  <si>
+    <t>1011</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>ARSH</t>
   </si>
   <si>
     <t>1010</t>
   </si>
   <si>
-    <t>ADDCUI</t>
-  </si>
-  <si>
-    <t>ALSH</t>
-  </si>
-  <si>
-    <t>ADDCI</t>
+    <t>ADD </t>
+  </si>
+  <si>
+    <t>1100</t>
+  </si>
+  <si>
+    <t>LSH</t>
+  </si>
+  <si>
+    <t>1101</t>
+  </si>
+  <si>
+    <t>MOV</t>
+  </si>
+  <si>
+    <t>RSH</t>
+  </si>
+  <si>
+    <t>1110</t>
+  </si>
+  <si>
+    <t>1111</t>
+  </si>
+  <si>
+    <t>nop</t>
+  </si>
+  <si>
+    <t>NOP</t>
+  </si>
+  <si>
+    <t>MOVIU</t>
   </si>
   <si>
     <t>xxxx</t>
   </si>
   <si>
-    <t>1000</t>
-  </si>
-  <si>
-    <t>ARSH</t>
-  </si>
-  <si>
-    <t>SUB</t>
-  </si>
-  <si>
-    <t>1001</t>
-  </si>
-  <si>
-    <t>SUBI</t>
-  </si>
-  <si>
-    <t>ADD </t>
-  </si>
-  <si>
-    <t>CMP</t>
-  </si>
-  <si>
-    <t>1011</t>
-  </si>
-  <si>
-    <t>CMPI</t>
-  </si>
-  <si>
-    <t>1100</t>
-  </si>
-  <si>
-    <t>LSH</t>
-  </si>
-  <si>
-    <t>CMPU/I</t>
-  </si>
-  <si>
-    <t>1101</t>
-  </si>
-  <si>
-    <t>MOV</t>
-  </si>
-  <si>
-    <t>1110</t>
-  </si>
-  <si>
-    <t>RSH</t>
-  </si>
-  <si>
-    <t>1111</t>
-  </si>
-  <si>
-    <t>NOP</t>
-  </si>
-  <si>
-    <t>LSHI</t>
-  </si>
-  <si>
     <t>LOAD</t>
   </si>
   <si>
+    <t>MOVI</t>
+  </si>
+  <si>
     <t>STORE</t>
   </si>
   <si>
-    <t>RSHI</t>
+    <t>Non-ALU instr</t>
   </si>
   <si>
     <t>BCOND</t>
@@ -199,34 +190,76 @@
     <t>JCOND</t>
   </si>
   <si>
+    <t>STOR</t>
+  </si>
+  <si>
     <t>JUMP</t>
   </si>
   <si>
-    <t>nop</t>
-  </si>
-  <si>
-    <t>MOVIU</t>
-  </si>
-  <si>
-    <t>MOVI</t>
+    <t>Jump</t>
+  </si>
+  <si>
+    <t>BGE</t>
   </si>
   <si>
     <t>MOVI </t>
   </si>
   <si>
-    <t>Non-ALU instr</t>
-  </si>
-  <si>
-    <t>STOR</t>
-  </si>
-  <si>
-    <t>Bcond</t>
-  </si>
-  <si>
-    <t>Jcond</t>
-  </si>
-  <si>
-    <t>Jump</t>
+    <t>BGEU</t>
+  </si>
+  <si>
+    <t>BEQ</t>
+  </si>
+  <si>
+    <t>BL</t>
+  </si>
+  <si>
+    <t>BLU</t>
+  </si>
+  <si>
+    <t>Instruction:</t>
+  </si>
+  <si>
+    <t>15:12</t>
+  </si>
+  <si>
+    <t>11:08</t>
+  </si>
+  <si>
+    <t>07:04</t>
+  </si>
+  <si>
+    <t>03:00</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>OpCode</t>
+  </si>
+  <si>
+    <t>OpExt</t>
+  </si>
+  <si>
+    <t>Src</t>
+  </si>
+  <si>
+    <t>Dst</t>
+  </si>
+  <si>
+    <t>Immediate</t>
+  </si>
+  <si>
+    <t>JumpBI / JumpFI</t>
+  </si>
+  <si>
+    <t>OpCode </t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>StorePC</t>
   </si>
 </sst>
 </file>
@@ -267,7 +300,7 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,12 +317,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="0023FF23"/>
         <bgColor rgb="003DEB3D"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF3366"/>
-        <bgColor rgb="00FF6600"/>
       </patternFill>
     </fill>
     <fill>
@@ -371,7 +398,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
@@ -386,10 +413,15 @@
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="0" numFmtId="165" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="4" fontId="0" numFmtId="165" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="0" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="6" fontId="0" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="7" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="8" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="9" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="6" fontId="4" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="7" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="8" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="165" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -403,7 +435,7 @@
     <indexedColors>
       <rgbColor rgb="00000000"/>
       <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF3366"/>
+      <rgbColor rgb="00FF0000"/>
       <rgbColor rgb="0023FF23"/>
       <rgbColor rgb="002300DC"/>
       <rgbColor rgb="00FFFF00"/>
@@ -467,7 +499,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
@@ -476,6 +508,7 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.1960784313725"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.6"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.73333333333333"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="1" width="9.05098039215686"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.1019607843137"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="30.4745098039216"/>
@@ -606,10 +639,10 @@
       <c r="A8" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="10" t="s">
+      <c r="B8" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E8" s="5"/>
@@ -622,11 +655,11 @@
       <c r="A9" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>10</v>
+      <c r="B9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="6" t="s">
@@ -638,31 +671,31 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="10">
       <c r="A10" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="6" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="11">
       <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>35</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="6" t="s">
@@ -674,137 +707,135 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="12">
       <c r="A12" s="8" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="6" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="13">
       <c r="A13" s="8" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="14">
       <c r="A14" s="8" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>42</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="G14" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="15">
       <c r="A15" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>16</v>
+        <v>27</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="6" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="16">
       <c r="A16" s="8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="17">
       <c r="A17" s="8" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="6" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="18">
       <c r="A18" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>17</v>
+        <v>33</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G18" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="19">
       <c r="A19" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>23</v>
+        <v>37</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>11</v>
@@ -813,18 +844,18 @@
         <v>16</v>
       </c>
       <c r="G19" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="20">
+      <c r="A20" s="8" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="20">
-      <c r="A20" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>26</v>
+      <c r="B20" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>17</v>
@@ -833,18 +864,18 @@
         <v>16</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="21">
       <c r="A21" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>23</v>
@@ -853,18 +884,18 @@
         <v>16</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="22">
       <c r="A22" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>35</v>
+        <v>49</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>26</v>
@@ -873,15 +904,15 @@
         <v>5</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="23">
+        <v>51</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="23">
       <c r="A23" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>50</v>
@@ -891,72 +922,68 @@
         <v>11</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="24">
-      <c r="A24" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>35</v>
-      </c>
+        <v>53</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="24">
+      <c r="A24" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
       <c r="E24" s="5"/>
       <c r="F24" s="6" t="s">
         <v>17</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="25">
-      <c r="A25" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>29</v>
+      <c r="A25" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>5</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="6" t="s">
         <v>23</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="26">
-      <c r="A26" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>36</v>
+      <c r="A26" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>11</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="27">
-      <c r="A27" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>16</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="27">
+      <c r="A27" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>26</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>10</v>
@@ -969,15 +996,8 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="28">
-      <c r="A28" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>48</v>
-      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
       <c r="E28" s="6" t="s">
         <v>22</v>
       </c>
@@ -988,36 +1008,25 @@
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="29">
-      <c r="A29" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>35</v>
-      </c>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="29">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
       <c r="E29" s="6" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>16</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="30">
-      <c r="A30" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>35</v>
-      </c>
+        <v>49</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="30">
+      <c r="A30" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
       <c r="E30" s="6" t="s">
         <v>36</v>
       </c>
@@ -1025,37 +1034,29 @@
         <v>16</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="31">
-      <c r="A31" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
+      <c r="A31" s="0" t="s">
+        <v>62</v>
+      </c>
       <c r="E31" s="6" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>16</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="32">
-      <c r="A32" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>5</v>
+      <c r="A32" s="0" t="s">
+        <v>63</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>16</v>
@@ -1066,38 +1067,26 @@
       <c r="I32" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="33">
-      <c r="A33" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>11</v>
+      <c r="A33" s="0" t="s">
+        <v>64</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>16</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="I33" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="34">
-      <c r="A34" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>17</v>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="34">
+      <c r="A34" s="0" t="s">
+        <v>65</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>16</v>
@@ -1107,18 +1096,9 @@
       </c>
       <c r="I34" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="35">
-      <c r="A35" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>23</v>
-      </c>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="35">
       <c r="E35" s="6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>16</v>
@@ -1129,17 +1109,8 @@
       <c r="I35" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="36">
-      <c r="A36" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="B36" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>26</v>
-      </c>
       <c r="E36" s="6" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>16</v>
@@ -1150,10 +1121,8 @@
       <c r="I36" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="37">
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
       <c r="E37" s="6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F37" s="6" t="s">
         <v>16</v>
@@ -1164,21 +1133,103 @@
       <c r="I37" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="38">
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
       <c r="I38" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="39">
-      <c r="A39" s="13"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
       <c r="I39" s="1"/>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="40">
+      <c r="I40" s="1"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="41">
+      <c r="A41" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E41" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="I41" s="1"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="42">
+      <c r="A42" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="43">
+      <c r="A43" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D43" s="15"/>
+      <c r="E43" s="16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="44">
+      <c r="A44" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="E44" s="15"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="45">
+      <c r="A45" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E45" s="16" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="E3:E18"/>
     <mergeCell ref="E22:E26"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="D44:E44"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Added mif file for blk mem
</commit_message>
<xml_diff>
--- a/documentation/OP_CODE.xlsx
+++ b/documentation/OP_CODE.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="81">
   <si>
     <t>OPCODE List</t>
   </si>
@@ -76,7 +76,7 @@
     <t>OR</t>
   </si>
   <si>
-    <t>MOVRET</t>
+    <t>JAL</t>
   </si>
   <si>
     <t>Copy return address from PC to reg</t>
@@ -103,94 +103,85 @@
     <t>NOT</t>
   </si>
   <si>
-    <t>ADDC</t>
+    <t>SUB</t>
+  </si>
+  <si>
+    <t>1001</t>
+  </si>
+  <si>
+    <t>SUBI</t>
+  </si>
+  <si>
+    <t>CMP</t>
   </si>
   <si>
     <t>0111</t>
   </si>
   <si>
-    <t>ADDCU</t>
+    <t>ALSH</t>
+  </si>
+  <si>
+    <t>CMPI</t>
+  </si>
+  <si>
+    <t>1011</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>ARSH</t>
   </si>
   <si>
     <t>1010</t>
   </si>
   <si>
-    <t>ADDCUI</t>
-  </si>
-  <si>
-    <t>ALSH</t>
-  </si>
-  <si>
-    <t>ADDCI</t>
+    <t>ADD </t>
+  </si>
+  <si>
+    <t>1100</t>
+  </si>
+  <si>
+    <t>LSH</t>
+  </si>
+  <si>
+    <t>1101</t>
+  </si>
+  <si>
+    <t>MOV</t>
+  </si>
+  <si>
+    <t>RSH</t>
+  </si>
+  <si>
+    <t>1110</t>
+  </si>
+  <si>
+    <t>1111</t>
+  </si>
+  <si>
+    <t>nop</t>
+  </si>
+  <si>
+    <t>NOP</t>
+  </si>
+  <si>
+    <t>MOVIU</t>
   </si>
   <si>
     <t>xxxx</t>
   </si>
   <si>
-    <t>1000</t>
-  </si>
-  <si>
-    <t>ARSH</t>
-  </si>
-  <si>
-    <t>SUB</t>
-  </si>
-  <si>
-    <t>1001</t>
-  </si>
-  <si>
-    <t>SUBI</t>
-  </si>
-  <si>
-    <t>ADD </t>
-  </si>
-  <si>
-    <t>CMP</t>
-  </si>
-  <si>
-    <t>1011</t>
-  </si>
-  <si>
-    <t>CMPI</t>
-  </si>
-  <si>
-    <t>1100</t>
-  </si>
-  <si>
-    <t>LSH</t>
-  </si>
-  <si>
-    <t>CMPU/I</t>
-  </si>
-  <si>
-    <t>1101</t>
-  </si>
-  <si>
-    <t>MOV</t>
-  </si>
-  <si>
-    <t>1110</t>
-  </si>
-  <si>
-    <t>RSH</t>
-  </si>
-  <si>
-    <t>1111</t>
-  </si>
-  <si>
-    <t>NOP</t>
-  </si>
-  <si>
-    <t>LSHI</t>
-  </si>
-  <si>
     <t>LOAD</t>
   </si>
   <si>
+    <t>MOVI</t>
+  </si>
+  <si>
     <t>STORE</t>
   </si>
   <si>
-    <t>RSHI</t>
+    <t>Non-ALU instr</t>
   </si>
   <si>
     <t>BCOND</t>
@@ -199,34 +190,76 @@
     <t>JCOND</t>
   </si>
   <si>
+    <t>STOR</t>
+  </si>
+  <si>
     <t>JUMP</t>
   </si>
   <si>
-    <t>nop</t>
-  </si>
-  <si>
-    <t>MOVIU</t>
-  </si>
-  <si>
-    <t>MOVI</t>
+    <t>Jump</t>
+  </si>
+  <si>
+    <t>BGE</t>
   </si>
   <si>
     <t>MOVI </t>
   </si>
   <si>
-    <t>Non-ALU instr</t>
-  </si>
-  <si>
-    <t>STOR</t>
-  </si>
-  <si>
-    <t>Bcond</t>
-  </si>
-  <si>
-    <t>Jcond</t>
-  </si>
-  <si>
-    <t>Jump</t>
+    <t>BGEU</t>
+  </si>
+  <si>
+    <t>BEQ</t>
+  </si>
+  <si>
+    <t>BL</t>
+  </si>
+  <si>
+    <t>BLU</t>
+  </si>
+  <si>
+    <t>Instruction:</t>
+  </si>
+  <si>
+    <t>15:12</t>
+  </si>
+  <si>
+    <t>11:08</t>
+  </si>
+  <si>
+    <t>07:04</t>
+  </si>
+  <si>
+    <t>03:00</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>OpCode</t>
+  </si>
+  <si>
+    <t>OpExt</t>
+  </si>
+  <si>
+    <t>Src</t>
+  </si>
+  <si>
+    <t>Dst</t>
+  </si>
+  <si>
+    <t>Immediate</t>
+  </si>
+  <si>
+    <t>JumpBI / JumpFI</t>
+  </si>
+  <si>
+    <t>OpCode </t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>StorePC</t>
   </si>
 </sst>
 </file>
@@ -267,7 +300,7 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,12 +317,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="0023FF23"/>
         <bgColor rgb="003DEB3D"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF3366"/>
-        <bgColor rgb="00FF6600"/>
       </patternFill>
     </fill>
     <fill>
@@ -371,7 +398,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
@@ -386,10 +413,15 @@
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="0" numFmtId="165" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="4" fontId="0" numFmtId="165" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="0" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="6" fontId="0" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="7" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="8" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="9" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="6" fontId="4" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="7" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="8" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="165" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -403,7 +435,7 @@
     <indexedColors>
       <rgbColor rgb="00000000"/>
       <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF3366"/>
+      <rgbColor rgb="00FF0000"/>
       <rgbColor rgb="0023FF23"/>
       <rgbColor rgb="002300DC"/>
       <rgbColor rgb="00FFFF00"/>
@@ -467,7 +499,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
@@ -476,6 +508,7 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.1960784313725"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.6"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.73333333333333"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="1" width="9.05098039215686"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.1019607843137"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="30.4745098039216"/>
@@ -606,10 +639,10 @@
       <c r="A8" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="10" t="s">
+      <c r="B8" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E8" s="5"/>
@@ -622,11 +655,11 @@
       <c r="A9" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>10</v>
+      <c r="B9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="E9" s="5"/>
       <c r="F9" s="6" t="s">
@@ -638,31 +671,31 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="10">
       <c r="A10" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="6" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="11">
       <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>35</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="6" t="s">
@@ -674,137 +707,135 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="12">
       <c r="A12" s="8" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="6" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="13">
       <c r="A13" s="8" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="14">
       <c r="A14" s="8" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>42</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="G14" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="15">
       <c r="A15" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>16</v>
+        <v>27</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="6" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="16">
       <c r="A16" s="8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="17">
       <c r="A17" s="8" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="6" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="18">
       <c r="A18" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>17</v>
+        <v>33</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G18" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="19">
       <c r="A19" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>23</v>
+        <v>37</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>11</v>
@@ -813,18 +844,18 @@
         <v>16</v>
       </c>
       <c r="G19" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="20">
+      <c r="A20" s="8" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="20">
-      <c r="A20" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>26</v>
+      <c r="B20" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>17</v>
@@ -833,18 +864,18 @@
         <v>16</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="21">
       <c r="A21" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>23</v>
@@ -853,18 +884,18 @@
         <v>16</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="22">
       <c r="A22" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>35</v>
+        <v>49</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>26</v>
@@ -873,15 +904,15 @@
         <v>5</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="23">
+        <v>51</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="23">
       <c r="A23" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>50</v>
@@ -891,72 +922,68 @@
         <v>11</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="24">
-      <c r="A24" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>35</v>
-      </c>
+        <v>53</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="24">
+      <c r="A24" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
       <c r="E24" s="5"/>
       <c r="F24" s="6" t="s">
         <v>17</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="25">
-      <c r="A25" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>29</v>
+      <c r="A25" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>5</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="6" t="s">
         <v>23</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="26">
-      <c r="A26" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>36</v>
+      <c r="A26" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>11</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="27">
-      <c r="A27" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>16</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="27">
+      <c r="A27" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>26</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>10</v>
@@ -969,15 +996,8 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="28">
-      <c r="A28" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>48</v>
-      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
       <c r="E28" s="6" t="s">
         <v>22</v>
       </c>
@@ -988,36 +1008,25 @@
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="29">
-      <c r="A29" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>35</v>
-      </c>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="29">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
       <c r="E29" s="6" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>16</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="30">
-      <c r="A30" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>35</v>
-      </c>
+        <v>49</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="30">
+      <c r="A30" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
       <c r="E30" s="6" t="s">
         <v>36</v>
       </c>
@@ -1025,37 +1034,29 @@
         <v>16</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="31">
-      <c r="A31" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
+      <c r="A31" s="0" t="s">
+        <v>62</v>
+      </c>
       <c r="E31" s="6" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>16</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="32">
-      <c r="A32" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>5</v>
+      <c r="A32" s="0" t="s">
+        <v>63</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>16</v>
@@ -1066,38 +1067,26 @@
       <c r="I32" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="33">
-      <c r="A33" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>11</v>
+      <c r="A33" s="0" t="s">
+        <v>64</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>16</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="I33" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="34">
-      <c r="A34" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>17</v>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="34">
+      <c r="A34" s="0" t="s">
+        <v>65</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>16</v>
@@ -1107,18 +1096,9 @@
       </c>
       <c r="I34" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="35">
-      <c r="A35" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>23</v>
-      </c>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="35">
       <c r="E35" s="6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>16</v>
@@ -1129,17 +1109,8 @@
       <c r="I35" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="36">
-      <c r="A36" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="B36" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>26</v>
-      </c>
       <c r="E36" s="6" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>16</v>
@@ -1150,10 +1121,8 @@
       <c r="I36" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="37">
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
       <c r="E37" s="6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F37" s="6" t="s">
         <v>16</v>
@@ -1164,21 +1133,103 @@
       <c r="I37" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="38">
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
       <c r="I38" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="39">
-      <c r="A39" s="13"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
       <c r="I39" s="1"/>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="40">
+      <c r="I40" s="1"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="41">
+      <c r="A41" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E41" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="I41" s="1"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="42">
+      <c r="A42" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="43">
+      <c r="A43" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D43" s="15"/>
+      <c r="E43" s="16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="44">
+      <c r="A44" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="E44" s="15"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="45">
+      <c r="A45" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E45" s="16" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="E3:E18"/>
     <mergeCell ref="E22:E26"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="D44:E44"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
modified opcode.xlsx for conditional instructions and fix mistake.
</commit_message>
<xml_diff>
--- a/documentation/OP_CODE.xlsx
+++ b/documentation/OP_CODE.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="80">
   <si>
     <t>OPCODE List</t>
   </si>
@@ -103,15 +103,51 @@
     <t>NOT</t>
   </si>
   <si>
+    <t>Instruction:</t>
+  </si>
+  <si>
+    <t>15:12</t>
+  </si>
+  <si>
+    <t>11:08</t>
+  </si>
+  <si>
+    <t>07:04</t>
+  </si>
+  <si>
+    <t>03:00</t>
+  </si>
+  <si>
     <t>SUB</t>
   </si>
   <si>
     <t>1001</t>
   </si>
   <si>
+    <t>ADD </t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>OpCode</t>
+  </si>
+  <si>
+    <t>OpExt</t>
+  </si>
+  <si>
+    <t>Src</t>
+  </si>
+  <si>
+    <t>Dst</t>
+  </si>
+  <si>
     <t>SUBI</t>
   </si>
   <si>
+    <t>Immediate</t>
+  </si>
+  <si>
     <t>CMP</t>
   </si>
   <si>
@@ -121,6 +157,9 @@
     <t>ALSH</t>
   </si>
   <si>
+    <t>JumpBI / JumpFI</t>
+  </si>
+  <si>
     <t>CMPI</t>
   </si>
   <si>
@@ -133,12 +172,18 @@
     <t>ARSH</t>
   </si>
   <si>
+    <t>OpCode </t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>StorePC</t>
+  </si>
+  <si>
     <t>1010</t>
   </si>
   <si>
-    <t>ADD </t>
-  </si>
-  <si>
     <t>1100</t>
   </si>
   <si>
@@ -160,106 +205,58 @@
     <t>1111</t>
   </si>
   <si>
+    <t>BGE</t>
+  </si>
+  <si>
     <t>nop</t>
   </si>
   <si>
+    <t>BGEU</t>
+  </si>
+  <si>
+    <t>BEQ</t>
+  </si>
+  <si>
+    <t>MOVIU</t>
+  </si>
+  <si>
+    <t>xxxx</t>
+  </si>
+  <si>
+    <t>BL</t>
+  </si>
+  <si>
+    <t>MOVI</t>
+  </si>
+  <si>
+    <t>BLU</t>
+  </si>
+  <si>
+    <t>Non-ALU instr</t>
+  </si>
+  <si>
     <t>NOP</t>
   </si>
   <si>
-    <t>MOVIU</t>
-  </si>
-  <si>
-    <t>xxxx</t>
-  </si>
-  <si>
     <t>LOAD</t>
   </si>
   <si>
-    <t>MOVI</t>
+    <t>STOR</t>
+  </si>
+  <si>
+    <t>Jump</t>
   </si>
   <si>
     <t>STORE</t>
   </si>
   <si>
-    <t>Non-ALU instr</t>
-  </si>
-  <si>
-    <t>BCOND</t>
-  </si>
-  <si>
-    <t>JCOND</t>
-  </si>
-  <si>
-    <t>STOR</t>
+    <t>MOVI </t>
+  </si>
+  <si>
+    <t>JGE</t>
   </si>
   <si>
     <t>JUMP</t>
-  </si>
-  <si>
-    <t>Jump</t>
-  </si>
-  <si>
-    <t>BGE</t>
-  </si>
-  <si>
-    <t>MOVI </t>
-  </si>
-  <si>
-    <t>BGEU</t>
-  </si>
-  <si>
-    <t>BEQ</t>
-  </si>
-  <si>
-    <t>BL</t>
-  </si>
-  <si>
-    <t>BLU</t>
-  </si>
-  <si>
-    <t>Instruction:</t>
-  </si>
-  <si>
-    <t>15:12</t>
-  </si>
-  <si>
-    <t>11:08</t>
-  </si>
-  <si>
-    <t>07:04</t>
-  </si>
-  <si>
-    <t>03:00</t>
-  </si>
-  <si>
-    <t>Register</t>
-  </si>
-  <si>
-    <t>OpCode</t>
-  </si>
-  <si>
-    <t>OpExt</t>
-  </si>
-  <si>
-    <t>Src</t>
-  </si>
-  <si>
-    <t>Dst</t>
-  </si>
-  <si>
-    <t>Immediate</t>
-  </si>
-  <si>
-    <t>JumpBI / JumpFI</t>
-  </si>
-  <si>
-    <t>OpCode </t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>StorePC</t>
   </si>
 </sst>
 </file>
@@ -398,7 +395,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
@@ -411,17 +408,18 @@
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="0" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="4" fontId="0" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="0" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="6" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="7" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="8" fontId="0" numFmtId="165" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="4" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="5" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="6" fontId="4" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="7" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="8" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -499,7 +497,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
@@ -511,6 +509,7 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.73333333333333"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="1" width="9.05098039215686"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.1019607843137"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.5137254901961"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="30.4745098039216"/>
   </cols>
   <sheetData>
@@ -634,29 +633,61 @@
       <c r="G7" s="7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="8">
+      <c r="I7" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="8">
       <c r="A8" s="8" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="7"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="9">
+      <c r="G8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="9">
       <c r="A9" s="8" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>16</v>
@@ -668,41 +699,82 @@
       <c r="G9" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="10">
+      <c r="I9" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="L9" s="10"/>
+      <c r="M9" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="10">
       <c r="A10" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="12" t="s">
         <v>16</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="6" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="11">
+        <v>45</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="M10" s="10"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="11">
       <c r="A11" s="8" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="6" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>37</v>
+        <v>50</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="M11" s="11" t="s">
+        <v>53</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="12">
@@ -717,10 +789,10 @@
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="6" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="13">
@@ -735,11 +807,9 @@
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>39</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="G13" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="14">
       <c r="A14" s="8" t="s">
@@ -753,7 +823,7 @@
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="6" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="G14" s="7"/>
     </row>
@@ -761,95 +831,95 @@
       <c r="A15" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="10" t="s">
+      <c r="B15" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="12" t="s">
         <v>26</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="6" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="16">
       <c r="A16" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>40</v>
+        <v>56</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>55</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="6" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="17">
       <c r="A17" s="8" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="6" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="18">
       <c r="A18" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>32</v>
+        <v>45</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>44</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="6" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="G18" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="19">
       <c r="A19" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>11</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="20">
       <c r="A20" s="8" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>17</v>
@@ -857,379 +927,335 @@
       <c r="C20" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>17</v>
-      </c>
+      <c r="E20" s="5"/>
       <c r="F20" s="6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="21">
       <c r="A21" s="8" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>23</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="E21" s="5"/>
       <c r="F21" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="22">
       <c r="A22" s="8" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>26</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="E22" s="5"/>
       <c r="F22" s="6" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="23">
       <c r="A23" s="8" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="6" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="24">
-      <c r="A24" s="12" t="s">
-        <v>54</v>
+      <c r="A24" s="14" t="s">
+        <v>71</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="E24" s="5"/>
+      <c r="E24" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="F24" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="25">
-      <c r="A25" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" s="14" t="s">
+      <c r="A25" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" s="5"/>
+      <c r="C25" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="F25" s="6" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="26">
-      <c r="A26" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="B26" s="14" t="s">
+      <c r="A26" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E26" s="5"/>
+      <c r="E26" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="F26" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="27">
+      <c r="A27" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="G26" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="27">
-      <c r="A27" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B27" s="14" t="s">
+      <c r="C27" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="E27" s="17"/>
       <c r="F27" s="6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="28">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="E28" s="6" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>16</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="29">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="E29" s="6" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>16</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="E30" s="6" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>16</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="31">
       <c r="A31" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>16</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="32">
       <c r="A32" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>16</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="I32" s="1"/>
+        <v>41</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="33">
       <c r="A33" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>35</v>
+        <v>68</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="I33" s="1"/>
+        <v>78</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="34">
       <c r="A34" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="E34" s="5"/>
+      <c r="F34" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="35">
+      <c r="E35" s="5"/>
+      <c r="F35" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G35" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E34" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G34" s="7" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="36">
+      <c r="E36" s="5"/>
+      <c r="F36" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="I36" s="1"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="37">
+      <c r="E37" s="5"/>
+      <c r="F37" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="I37" s="1"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="38">
+      <c r="E38" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I38" s="1"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="39">
+      <c r="E39" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="I39" s="1"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="40">
+      <c r="E40" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G40" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I34" s="1"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="35">
-      <c r="E35" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G35" s="7" t="s">
+      <c r="I40" s="1"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="41">
+      <c r="E41" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G41" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I35" s="1"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="36">
-      <c r="E36" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G36" s="7" t="s">
+      <c r="I41" s="1"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="42">
+      <c r="E42" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G42" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I36" s="1"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="37">
-      <c r="E37" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G37" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="I37" s="1"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="38">
-      <c r="I38" s="1"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="39">
-      <c r="I39" s="1"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="40">
-      <c r="I40" s="1"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="41">
-      <c r="A41" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="B41" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="C41" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="D41" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="E41" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="I41" s="1"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="42">
-      <c r="A42" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B42" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="C42" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D42" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="E42" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="43">
-      <c r="A43" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="C43" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="D43" s="15"/>
-      <c r="E43" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="44">
-      <c r="A44" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="B44" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="C44" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D44" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="E44" s="15"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="45">
-      <c r="A45" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B45" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="C45" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D45" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="E45" s="16" t="s">
-        <v>80</v>
-      </c>
+      <c r="I42" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="E3:E18"/>
-    <mergeCell ref="E22:E26"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="E19:E23"/>
+    <mergeCell ref="E33:E37"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
modified the opcodes file again
</commit_message>
<xml_diff>
--- a/documentation/OP_CODE.xlsx
+++ b/documentation/OP_CODE.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="87">
   <si>
     <t>OPCODE List</t>
   </si>
@@ -181,9 +181,18 @@
     <t>StorePC</t>
   </si>
   <si>
+    <t>Load</t>
+  </si>
+  <si>
+    <t>StoreTo</t>
+  </si>
+  <si>
     <t>1010</t>
   </si>
   <si>
+    <t>Store</t>
+  </si>
+  <si>
     <t>1100</t>
   </si>
   <si>
@@ -254,6 +263,18 @@
   </si>
   <si>
     <t>JGE</t>
+  </si>
+  <si>
+    <t>JGEU</t>
+  </si>
+  <si>
+    <t>JEQ</t>
+  </si>
+  <si>
+    <t>JL</t>
+  </si>
+  <si>
+    <t>JLU</t>
   </si>
   <si>
     <t>JUMP</t>
@@ -777,7 +798,7 @@
         <v>53</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="12">
       <c r="A12" s="8" t="s">
         <v>12</v>
       </c>
@@ -794,8 +815,23 @@
       <c r="G12" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="13">
+      <c r="I12" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="13">
       <c r="A13" s="8" t="s">
         <v>18</v>
       </c>
@@ -807,9 +843,24 @@
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G13" s="7"/>
+      <c r="I13" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="L13" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="14">
       <c r="A14" s="8" t="s">
@@ -839,46 +890,46 @@
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="16">
       <c r="A16" s="8" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="6" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="17">
       <c r="A17" s="8" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="6" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="18">
@@ -893,7 +944,7 @@
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="6" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="G18" s="7"/>
     </row>
@@ -914,12 +965,12 @@
         <v>5</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="20">
       <c r="A20" s="8" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>17</v>
@@ -932,66 +983,66 @@
         <v>11</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="21">
       <c r="A21" s="8" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="6" t="s">
         <v>17</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="22">
       <c r="A22" s="8" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>44</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="6" t="s">
         <v>23</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="23">
       <c r="A23" s="8" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>49</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="24">
       <c r="A24" s="14" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1002,12 +1053,12 @@
         <v>16</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="25">
       <c r="A25" s="15" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B25" s="16" t="s">
         <v>26</v>
@@ -1027,7 +1078,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="26">
       <c r="A26" s="15" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B26" s="16" t="s">
         <v>26</v>
@@ -1042,12 +1093,12 @@
         <v>5</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="27">
       <c r="A27" s="15" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B27" s="16" t="s">
         <v>26</v>
@@ -1060,7 +1111,7 @@
         <v>11</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="28">
@@ -1091,7 +1142,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1102,12 +1153,12 @@
         <v>16</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="31">
       <c r="A31" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>49</v>
@@ -1116,12 +1167,12 @@
         <v>16</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="32">
       <c r="A32" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>34</v>
@@ -1135,28 +1186,28 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="33">
       <c r="A33" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>5</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="34">
       <c r="A34" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="6" t="s">
         <v>11</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="35">
@@ -1165,7 +1216,7 @@
         <v>17</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="36">
@@ -1174,7 +1225,7 @@
         <v>23</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="I36" s="1"/>
     </row>
@@ -1184,7 +1235,7 @@
         <v>26</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="I37" s="1"/>
     </row>
@@ -1202,19 +1253,19 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="39">
       <c r="E39" s="6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>16</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="I39" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="40">
       <c r="E40" s="6" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>16</v>
@@ -1226,7 +1277,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="41">
       <c r="E41" s="6" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>16</v>
@@ -1238,7 +1289,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="42">
       <c r="E42" s="6" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F42" s="6" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
added branching instructions modified opcode mnemonics
</commit_message>
<xml_diff>
--- a/documentation/OP_CODE.xlsx
+++ b/documentation/OP_CODE.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="90">
   <si>
     <t>OPCODE List</t>
   </si>
@@ -220,61 +220,70 @@
     <t>nop</t>
   </si>
   <si>
+    <t>BHG</t>
+  </si>
+  <si>
+    <t>BEQ</t>
+  </si>
+  <si>
+    <t>MOVIU</t>
+  </si>
+  <si>
+    <t>xxxx</t>
+  </si>
+  <si>
+    <t>BLT</t>
+  </si>
+  <si>
+    <t>MOVI</t>
+  </si>
+  <si>
+    <t>BLS</t>
+  </si>
+  <si>
+    <t>Non-ALU instr</t>
+  </si>
+  <si>
+    <t>NOP</t>
+  </si>
+  <si>
+    <t>LOAD</t>
+  </si>
+  <si>
+    <t>STOR</t>
+  </si>
+  <si>
+    <t>Jump</t>
+  </si>
+  <si>
+    <t>STORE</t>
+  </si>
+  <si>
     <t>BGEU</t>
   </si>
   <si>
-    <t>BEQ</t>
-  </si>
-  <si>
-    <t>MOVIU</t>
-  </si>
-  <si>
-    <t>xxxx</t>
+    <t>MOVI </t>
   </si>
   <si>
     <t>BL</t>
   </si>
   <si>
-    <t>MOVI</t>
+    <t>JGE</t>
   </si>
   <si>
     <t>BLU</t>
   </si>
   <si>
-    <t>Non-ALU instr</t>
-  </si>
-  <si>
-    <t>NOP</t>
-  </si>
-  <si>
-    <t>LOAD</t>
-  </si>
-  <si>
-    <t>STOR</t>
-  </si>
-  <si>
-    <t>Jump</t>
-  </si>
-  <si>
-    <t>STORE</t>
-  </si>
-  <si>
-    <t>MOVI </t>
-  </si>
-  <si>
-    <t>JGE</t>
-  </si>
-  <si>
-    <t>JGEU</t>
+    <t>JHG</t>
   </si>
   <si>
     <t>JEQ</t>
   </si>
   <si>
-    <t>JL</t>
-  </si>
-  <si>
-    <t>JLU</t>
+    <t>JLT</t>
+  </si>
+  <si>
+    <t>JLS</t>
   </si>
   <si>
     <t>JUMP</t>
@@ -1158,7 +1167,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="31">
       <c r="A31" s="0" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>49</v>
@@ -1167,7 +1176,7 @@
         <v>16</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="32">
@@ -1186,7 +1195,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="33">
       <c r="A33" s="0" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>56</v>
@@ -1195,19 +1204,19 @@
         <v>5</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="34">
       <c r="A34" s="0" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="6" t="s">
         <v>11</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="35">
@@ -1216,7 +1225,7 @@
         <v>17</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="36">
@@ -1225,7 +1234,7 @@
         <v>23</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="I36" s="1"/>
     </row>
@@ -1235,7 +1244,7 @@
         <v>26</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="I37" s="1"/>
     </row>
@@ -1259,7 +1268,7 @@
         <v>16</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="I39" s="1"/>
     </row>

</xml_diff>

<commit_message>
Added Jump, StorePC, JCond, instructions and changed pc to increment as signed values
</commit_message>
<xml_diff>
--- a/documentation/OP_CODE.xlsx
+++ b/documentation/OP_CODE.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="92">
   <si>
     <t>OPCODE List</t>
   </si>
@@ -157,7 +157,7 @@
     <t>ALSH</t>
   </si>
   <si>
-    <t>JumpBI / JumpFI</t>
+    <t>JCOND</t>
   </si>
   <si>
     <t>CMPI</t>
@@ -172,18 +172,24 @@
     <t>ARSH</t>
   </si>
   <si>
+    <t>STOREPC</t>
+  </si>
+  <si>
     <t>OpCode </t>
   </si>
   <si>
+    <t>xxxx</t>
+  </si>
+  <si>
+    <t>StorePC</t>
+  </si>
+  <si>
+    <t>Load</t>
+  </si>
+  <si>
     <t>Address</t>
   </si>
   <si>
-    <t>StorePC</t>
-  </si>
-  <si>
-    <t>Load</t>
-  </si>
-  <si>
     <t>StoreTo</t>
   </si>
   <si>
@@ -193,6 +199,9 @@
     <t>Store</t>
   </si>
   <si>
+    <t>JUMP </t>
+  </si>
+  <si>
     <t>1100</t>
   </si>
   <si>
@@ -227,9 +236,6 @@
   </si>
   <si>
     <t>MOVIU</t>
-  </si>
-  <si>
-    <t>xxxx</t>
   </si>
   <si>
     <t>BLT</t>
@@ -527,7 +533,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M42"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
@@ -792,19 +798,19 @@
         <v>50</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K11" s="10" t="s">
         <v>38</v>
       </c>
       <c r="L11" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="M11" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="12">
@@ -825,7 +831,7 @@
         <v>33</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J12" s="10" t="s">
         <v>37</v>
@@ -834,10 +840,10 @@
         <v>38</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="M12" s="10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="13">
@@ -852,11 +858,11 @@
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G13" s="7"/>
       <c r="I13" s="10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J13" s="10" t="s">
         <v>37</v>
@@ -865,13 +871,13 @@
         <v>38</v>
       </c>
       <c r="L13" s="10" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="M13" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="14">
+        <v>57</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="14">
       <c r="A14" s="8" t="s">
         <v>24</v>
       </c>
@@ -886,6 +892,21 @@
         <v>48</v>
       </c>
       <c r="G14" s="7"/>
+      <c r="I14" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="L14" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="M14" s="10" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="15">
       <c r="A15" s="8" t="s">
@@ -899,46 +920,46 @@
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="6" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="16">
       <c r="A16" s="8" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="6" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="17">
       <c r="A17" s="8" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="18">
@@ -953,7 +974,7 @@
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="6" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G18" s="7"/>
     </row>
@@ -974,12 +995,12 @@
         <v>5</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="20">
       <c r="A20" s="8" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>17</v>
@@ -992,66 +1013,66 @@
         <v>11</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="21">
       <c r="A21" s="8" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="6" t="s">
         <v>17</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="22">
       <c r="A22" s="8" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>44</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="6" t="s">
         <v>23</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="23">
       <c r="A23" s="8" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>49</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="24">
       <c r="A24" s="14" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1062,12 +1083,12 @@
         <v>16</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="25">
       <c r="A25" s="15" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B25" s="16" t="s">
         <v>26</v>
@@ -1087,7 +1108,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="26">
       <c r="A26" s="15" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B26" s="16" t="s">
         <v>26</v>
@@ -1102,12 +1123,12 @@
         <v>5</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="27">
       <c r="A27" s="15" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B27" s="16" t="s">
         <v>26</v>
@@ -1120,7 +1141,7 @@
         <v>11</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="28">
@@ -1151,7 +1172,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1162,12 +1183,12 @@
         <v>16</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="31">
       <c r="A31" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>49</v>
@@ -1176,12 +1197,12 @@
         <v>16</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="32">
       <c r="A32" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>34</v>
@@ -1195,28 +1216,28 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="33">
       <c r="A33" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>5</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="34">
       <c r="A34" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="6" t="s">
         <v>11</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="35">
@@ -1225,7 +1246,7 @@
         <v>17</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="36">
@@ -1234,7 +1255,7 @@
         <v>23</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="I36" s="1"/>
     </row>
@@ -1244,7 +1265,7 @@
         <v>26</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I37" s="1"/>
     </row>
@@ -1261,26 +1282,24 @@
       <c r="I38" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="39">
-      <c r="E39" s="6" t="s">
-        <v>58</v>
+      <c r="E39" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I39" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="40">
-      <c r="E40" s="6" t="s">
-        <v>60</v>
-      </c>
+      <c r="E40" s="5"/>
       <c r="F40" s="6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="I40" s="1"/>
     </row>
@@ -1298,7 +1317,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="42">
       <c r="E42" s="6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F42" s="6" t="s">
         <v>16</v>
@@ -1308,14 +1327,27 @@
       </c>
       <c r="I42" s="1"/>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="43">
+      <c r="E43" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I43" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="E3:E18"/>
     <mergeCell ref="K9:L9"/>
     <mergeCell ref="L10:M10"/>
     <mergeCell ref="E19:E23"/>
     <mergeCell ref="E33:E37"/>
+    <mergeCell ref="E39:E40"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Fixed the ALU and CPU Controller to use CLFZN instead of CZLFN...
</commit_message>
<xml_diff>
--- a/documentation/OP_CODE.xlsx
+++ b/documentation/OP_CODE.xlsx
@@ -229,7 +229,7 @@
     <t>nop</t>
   </si>
   <si>
-    <t>BHG</t>
+    <t>BHS</t>
   </si>
   <si>
     <t>BEQ</t>
@@ -280,7 +280,7 @@
     <t>BLU</t>
   </si>
   <si>
-    <t>JHG</t>
+    <t>JHS</t>
   </si>
   <si>
     <t>JEQ</t>

</xml_diff>

<commit_message>
Changed the operation of conditional jumps to increment PC by offset when true.
</commit_message>
<xml_diff>
--- a/documentation/OP_CODE.xlsx
+++ b/documentation/OP_CODE.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="93">
   <si>
     <t>OPCODE List</t>
   </si>
@@ -290,6 +290,9 @@
   </si>
   <si>
     <t>JLS</t>
+  </si>
+  <si>
+    <t>JOFFSET</t>
   </si>
   <si>
     <t>JUMP</t>
@@ -533,7 +536,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M43"/>
+  <dimension ref="A1:M44"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
@@ -1270,54 +1273,52 @@
       <c r="I37" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="38">
-      <c r="E38" s="6" t="s">
+      <c r="E38" s="5"/>
+      <c r="F38" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="I38" s="1"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="39">
+      <c r="E39" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F38" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G38" s="7" t="s">
+      <c r="F39" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G39" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="I38" s="1"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="39">
-      <c r="E39" s="5" t="s">
+      <c r="I39" s="1"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="40">
+      <c r="E40" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F39" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G39" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="I39" s="1"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="40">
-      <c r="E40" s="5"/>
       <c r="F40" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="I40" s="1"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="41">
+      <c r="E41" s="5"/>
+      <c r="F41" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G40" s="7" t="s">
+      <c r="G41" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="I40" s="1"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="41">
-      <c r="E41" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G41" s="7" t="s">
-        <v>6</v>
       </c>
       <c r="I41" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="42">
       <c r="E42" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F42" s="6" t="s">
         <v>16</v>
@@ -1329,7 +1330,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="43">
       <c r="E43" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>16</v>
@@ -1338,6 +1339,18 @@
         <v>6</v>
       </c>
       <c r="I43" s="1"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="44">
+      <c r="E44" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I44" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1346,8 +1359,8 @@
     <mergeCell ref="K9:L9"/>
     <mergeCell ref="L10:M10"/>
     <mergeCell ref="E19:E23"/>
-    <mergeCell ref="E33:E37"/>
-    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="E33:E38"/>
+    <mergeCell ref="E40:E41"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Added final (hopefully) instructions to opcode.xlsx
</commit_message>
<xml_diff>
--- a/documentation/OP_CODE.xlsx
+++ b/documentation/OP_CODE.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="98">
   <si>
     <t>OPCODE List</t>
   </si>
@@ -208,22 +208,37 @@
     <t>LSH</t>
   </si>
   <si>
+    <t>SETBEGINVGA</t>
+  </si>
+  <si>
     <t>1101</t>
   </si>
   <si>
     <t>MOV</t>
   </si>
   <si>
+    <t>SETROWVGA</t>
+  </si>
+  <si>
     <t>RSH</t>
   </si>
   <si>
     <t>1110</t>
   </si>
   <si>
+    <t>READSERIAL</t>
+  </si>
+  <si>
     <t>1111</t>
   </si>
   <si>
+    <t>WRITESERIAL</t>
+  </si>
+  <si>
     <t>BGE</t>
+  </si>
+  <si>
+    <t>READGAMEPAD</t>
   </si>
   <si>
     <t>nop</t>
@@ -536,7 +551,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M44"/>
+  <dimension ref="A1:M48"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
@@ -911,7 +926,7 @@
         <v>53</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="15">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="15">
       <c r="A15" s="8" t="s">
         <v>27</v>
       </c>
@@ -928,8 +943,23 @@
       <c r="G15" s="7" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="16">
+      <c r="I15" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="L15" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="16">
       <c r="A16" s="8" t="s">
         <v>62</v>
       </c>
@@ -941,31 +971,61 @@
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="17">
+        <v>65</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="L16" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="M16" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="17">
       <c r="A17" s="8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="18">
+        <v>67</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="L17" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="M17" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="18">
       <c r="A18" s="8" t="s">
         <v>45</v>
       </c>
@@ -977,11 +1037,26 @@
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="6" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G18" s="7"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="19">
+      <c r="I18" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="L18" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="M18" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="19">
       <c r="A19" s="8" t="s">
         <v>50</v>
       </c>
@@ -998,12 +1073,27 @@
         <v>5</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>68</v>
+        <v>72</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K19" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="L19" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="M19" s="10" t="s">
+        <v>40</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="20">
       <c r="A20" s="8" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>17</v>
@@ -1016,30 +1106,30 @@
         <v>11</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="21">
       <c r="A21" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>64</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>63</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="6" t="s">
         <v>17</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="22">
       <c r="A22" s="8" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>44</v>
@@ -1052,12 +1142,12 @@
         <v>23</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="23">
       <c r="A23" s="8" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>49</v>
@@ -1070,12 +1160,12 @@
         <v>26</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="24">
       <c r="A24" s="14" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1086,12 +1176,12 @@
         <v>16</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="25">
       <c r="A25" s="15" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B25" s="16" t="s">
         <v>26</v>
@@ -1111,7 +1201,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="26">
       <c r="A26" s="15" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B26" s="16" t="s">
         <v>26</v>
@@ -1126,12 +1216,12 @@
         <v>5</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="27">
       <c r="A27" s="15" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B27" s="16" t="s">
         <v>26</v>
@@ -1144,7 +1234,7 @@
         <v>11</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="28">
@@ -1175,7 +1265,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1186,12 +1276,12 @@
         <v>16</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="31">
       <c r="A31" s="0" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>49</v>
@@ -1200,12 +1290,12 @@
         <v>16</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="32">
       <c r="A32" s="0" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>34</v>
@@ -1219,7 +1309,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="33">
       <c r="A33" s="0" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>58</v>
@@ -1228,19 +1318,19 @@
         <v>5</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="34">
       <c r="A34" s="0" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="6" t="s">
         <v>11</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="35">
@@ -1249,7 +1339,7 @@
         <v>17</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="36">
@@ -1258,7 +1348,7 @@
         <v>23</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="I36" s="1"/>
     </row>
@@ -1268,7 +1358,7 @@
         <v>26</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="I37" s="1"/>
     </row>
@@ -1278,7 +1368,7 @@
         <v>10</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="I38" s="1"/>
     </row>
@@ -1302,7 +1392,7 @@
         <v>5</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="I40" s="1"/>
     </row>
@@ -1317,43 +1407,80 @@
       <c r="I41" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="42">
-      <c r="E42" s="6" t="s">
+      <c r="E42" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G42" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F42" s="6" t="s">
+      <c r="I42" s="1"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="43">
+      <c r="E43" s="5"/>
+      <c r="F43" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="I43" s="1"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="44">
+      <c r="E44" s="5"/>
+      <c r="F44" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I44" s="1"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="45">
+      <c r="E45" s="5"/>
+      <c r="F45" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="I45" s="1"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="46">
+      <c r="E46" s="5"/>
+      <c r="F46" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="47">
+      <c r="E47" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F47" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G42" s="7" t="s">
+      <c r="G47" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I42" s="1"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="43">
-      <c r="E43" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F43" s="6" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="48">
+      <c r="E48" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F48" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G43" s="7" t="s">
+      <c r="G48" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I43" s="1"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="44">
-      <c r="E44" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G44" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="I44" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="E3:E18"/>
     <mergeCell ref="K9:L9"/>
@@ -1361,6 +1488,7 @@
     <mergeCell ref="E19:E23"/>
     <mergeCell ref="E33:E38"/>
     <mergeCell ref="E40:E41"/>
+    <mergeCell ref="E42:E46"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Added system clock to cpu, and CLOCK instruction to read it.
</commit_message>
<xml_diff>
--- a/documentation/OP_CODE.xlsx
+++ b/documentation/OP_CODE.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="95">
   <si>
     <t>OPCODE List</t>
   </si>
@@ -124,9 +124,6 @@
     <t>1001</t>
   </si>
   <si>
-    <t>ADD </t>
-  </si>
-  <si>
     <t>Register</t>
   </si>
   <si>
@@ -175,9 +172,6 @@
     <t>STOREPC</t>
   </si>
   <si>
-    <t>OpCode </t>
-  </si>
-  <si>
     <t>xxxx</t>
   </si>
   <si>
@@ -199,7 +193,7 @@
     <t>Store</t>
   </si>
   <si>
-    <t>JUMP </t>
+    <t>JUMP</t>
   </si>
   <si>
     <t>1100</t>
@@ -247,6 +241,9 @@
     <t>BHS</t>
   </si>
   <si>
+    <t>CLOCK</t>
+  </si>
+  <si>
     <t>BEQ</t>
   </si>
   <si>
@@ -283,9 +280,6 @@
     <t>BGEU</t>
   </si>
   <si>
-    <t>MOVI </t>
-  </si>
-  <si>
     <t>BL</t>
   </si>
   <si>
@@ -308,9 +302,6 @@
   </si>
   <si>
     <t>JOFFSET</t>
-  </si>
-  <si>
-    <t>JUMP</t>
   </si>
 </sst>
 </file>
@@ -453,7 +444,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
@@ -551,20 +542,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M48"/>
+  <dimension ref="A1:M49"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.1960784313725"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.6"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.73333333333333"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="9.05098039215686"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.1019607843137"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.5137254901961"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="30.4745098039216"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2509803921569"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.63137254901961"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.76862745098039"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="9.09411764705882"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.156862745098"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.5921568627451"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="30.6"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.54117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1">
@@ -578,7 +572,7 @@
       </c>
       <c r="J2" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="3">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -604,7 +598,7 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="4">
       <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
@@ -628,7 +622,7 @@
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="5">
       <c r="A5" s="8" t="s">
         <v>15</v>
       </c>
@@ -652,7 +646,7 @@
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="6">
       <c r="A6" s="8" t="s">
         <v>21</v>
       </c>
@@ -670,7 +664,7 @@
         <v>24</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="7">
       <c r="A7" s="8" t="s">
         <v>25</v>
       </c>
@@ -703,7 +697,7 @@
         <v>32</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="8">
       <c r="A8" s="8" t="s">
         <v>33</v>
       </c>
@@ -718,27 +712,27 @@
         <v>10</v>
       </c>
       <c r="G8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="J8" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="K8" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="K8" s="10" t="s">
+      <c r="L8" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="M8" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="M8" s="11" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="9">
+      <c r="A9" s="8" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="9">
-      <c r="A9" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>34</v>
@@ -754,22 +748,22 @@
         <v>21</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L9" s="10"/>
       <c r="M9" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="10">
+        <v>39</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="10">
       <c r="A10" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>23</v>
@@ -779,59 +773,59 @@
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="I10" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="I10" s="10" t="s">
+      <c r="J10" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="M10" s="10"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="11">
+      <c r="A11" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="J10" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="K10" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="L10" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="M10" s="10"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="11">
-      <c r="A11" s="8" t="s">
+      <c r="B11" s="9" t="s">
         <v>47</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>48</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="I11" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="I11" s="10" t="s">
+      <c r="J11" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="L11" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="J11" s="10" t="s">
+      <c r="M11" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="K11" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="L11" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="M11" s="11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="12">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="12">
       <c r="A12" s="8" t="s">
         <v>12</v>
       </c>
@@ -849,22 +843,22 @@
         <v>33</v>
       </c>
       <c r="I12" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="M12" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="J12" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="K12" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="L12" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="M12" s="10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="13">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="13">
       <c r="A13" s="8" t="s">
         <v>18</v>
       </c>
@@ -876,26 +870,26 @@
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G13" s="7"/>
       <c r="I13" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K13" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="K13" s="10" t="s">
-        <v>38</v>
-      </c>
       <c r="L13" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M13" s="10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="14">
+        <v>55</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="14">
       <c r="A14" s="8" t="s">
         <v>24</v>
       </c>
@@ -907,26 +901,26 @@
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G14" s="7"/>
       <c r="I14" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K14" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="K14" s="10" t="s">
-        <v>38</v>
-      </c>
       <c r="L14" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M14" s="10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="15">
+        <v>51</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="15">
       <c r="A15" s="8" t="s">
         <v>27</v>
       </c>
@@ -938,133 +932,133 @@
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="G15" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="I15" s="10" t="s">
-        <v>63</v>
-      </c>
       <c r="J15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K15" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="K15" s="10" t="s">
+      <c r="L15" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="L15" s="10" t="s">
-        <v>39</v>
-      </c>
       <c r="M15" s="10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="16">
+        <v>51</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="16">
       <c r="A16" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I16" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="J16" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="L16" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="M16" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="17">
+      <c r="A17" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="I16" s="10" t="s">
+      <c r="B17" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="J16" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="K16" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="L16" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="M16" s="10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="17">
-      <c r="A17" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>68</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G17" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I17" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="I17" s="10" t="s">
-        <v>69</v>
-      </c>
       <c r="J17" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K17" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="K17" s="10" t="s">
-        <v>38</v>
-      </c>
       <c r="L17" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="M17" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="18">
+        <v>39</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="18">
       <c r="A18" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G18" s="7"/>
       <c r="I18" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J18" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K18" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="K18" s="10" t="s">
+      <c r="L18" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="L18" s="10" t="s">
-        <v>39</v>
-      </c>
       <c r="M18" s="10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="19">
+        <v>51</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="19">
       <c r="A19" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>11</v>
@@ -1073,27 +1067,27 @@
         <v>5</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J19" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K19" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="K19" s="10" t="s">
-        <v>38</v>
-      </c>
       <c r="L19" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="M19" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="20">
       <c r="A20" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>17</v>
@@ -1106,66 +1100,81 @@
         <v>11</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="21">
+        <v>73</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K20" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="L20" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="M20" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="21">
       <c r="A21" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="6" t="s">
         <v>17</v>
       </c>
       <c r="G21" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="22">
+      <c r="A22" s="8" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="22">
-      <c r="A22" s="8" t="s">
-        <v>77</v>
-      </c>
       <c r="B22" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="6" t="s">
         <v>23</v>
       </c>
       <c r="G22" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="23">
+      <c r="A23" s="8" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="23">
-      <c r="A23" s="8" t="s">
-        <v>79</v>
-      </c>
       <c r="B23" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G23" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="24">
+      <c r="A24" s="14" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="24">
-      <c r="A24" s="14" t="s">
-        <v>81</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1176,12 +1185,12 @@
         <v>16</v>
       </c>
       <c r="G24" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="25">
+      <c r="A25" s="15" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="25">
-      <c r="A25" s="15" t="s">
-        <v>83</v>
       </c>
       <c r="B25" s="16" t="s">
         <v>26</v>
@@ -1196,12 +1205,12 @@
         <v>16</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="26">
+        <v>42</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="26">
       <c r="A26" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B26" s="16" t="s">
         <v>26</v>
@@ -1216,12 +1225,12 @@
         <v>5</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="27">
+        <v>82</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="27">
       <c r="A27" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B27" s="16" t="s">
         <v>26</v>
@@ -1234,10 +1243,10 @@
         <v>11</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="28">
+        <v>85</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="28">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="E28" s="6" t="s">
@@ -1250,7 +1259,7 @@
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="29">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="29">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="E29" s="6" t="s">
@@ -1263,39 +1272,39 @@
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="30">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="E30" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>16</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="31">
+        <v>76</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="31">
       <c r="A31" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>16</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="32">
+        <v>78</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="32">
       <c r="A32" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>34</v>
@@ -1304,178 +1313,187 @@
         <v>16</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="33">
+        <v>40</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="33">
       <c r="A33" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="34">
+      <c r="A34" s="0" t="s">
         <v>89</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="34">
-      <c r="A34" s="0" t="s">
-        <v>91</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="6" t="s">
         <v>11</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="35">
+        <v>90</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="35">
       <c r="E35" s="5"/>
       <c r="F35" s="6" t="s">
         <v>17</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="36">
+        <v>91</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="36">
       <c r="E36" s="5"/>
       <c r="F36" s="6" t="s">
         <v>23</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I36" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="37">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="37">
       <c r="E37" s="5"/>
       <c r="F37" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I37" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="38">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="38">
       <c r="E38" s="5"/>
       <c r="F38" s="6" t="s">
         <v>10</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I38" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="39">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="39">
       <c r="E39" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>16</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I39" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="40">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="40">
       <c r="E40" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>5</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>97</v>
+        <v>58</v>
       </c>
       <c r="I40" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="41">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="41">
       <c r="E41" s="5"/>
       <c r="F41" s="6" t="s">
         <v>11</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I41" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="42">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="42">
       <c r="E42" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F42" s="6" t="s">
         <v>5</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I42" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="43">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="43">
       <c r="E43" s="5"/>
       <c r="F43" s="6" t="s">
         <v>11</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I43" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="44">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="44">
       <c r="E44" s="5"/>
       <c r="F44" s="6" t="s">
         <v>17</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I44" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="45">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="45">
       <c r="E45" s="5"/>
       <c r="F45" s="6" t="s">
         <v>23</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I45" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="46">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="46">
       <c r="E46" s="5"/>
       <c r="F46" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="47">
-      <c r="E47" s="6" t="s">
-        <v>68</v>
-      </c>
+        <v>71</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="47">
+      <c r="E47" s="5"/>
       <c r="F47" s="6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.1" outlineLevel="0" r="48">
+        <v>74</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="48">
       <c r="E48" s="6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F48" s="6" t="s">
         <v>16</v>
       </c>
       <c r="G48" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="49">
+      <c r="E49" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G49" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1492,7 +1510,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="landscape" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1511,6 +1529,9 @@
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.54117647058824"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1533,6 +1554,9 @@
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.54117647058824"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>